<commit_message>
Refactor + Excel improvement + Usability improvements
</commit_message>
<xml_diff>
--- a/Documents/FileSystem_commands.xlsx
+++ b/Documents/FileSystem_commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j00914576\Desktop\Code\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7646BC91-05ED-4B4C-B2EA-2B6517BB475E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B580B8C3-6A46-4993-84D1-DB30403E8751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>name</t>
   </si>
@@ -191,52 +191,49 @@
     <t>fs_layer_distribution_algorithm</t>
   </si>
   <si>
+    <t>file_system_name</t>
+  </si>
+  <si>
+    <t>filter_name</t>
+  </si>
+  <si>
+    <t>filter_storage_pool_id</t>
+  </si>
+  <si>
+    <t>filter_health_status</t>
+  </si>
+  <si>
+    <t>filter_running_status</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>sort_by</t>
+  </si>
+  <si>
+    <t>sort_mode</t>
+  </si>
+  <si>
+    <t>file_system_id_list</t>
+  </si>
+  <si>
+    <t>file_system_name_list</t>
+  </si>
+  <si>
+    <t>vstore_id</t>
+  </si>
+  <si>
     <t>fs1</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
     <t>sp1</t>
-  </si>
-  <si>
-    <t>file_system_name</t>
-  </si>
-  <si>
-    <t>filter_name</t>
-  </si>
-  <si>
-    <t>filter_storage_pool_id</t>
-  </si>
-  <si>
-    <t>filter_health_status</t>
-  </si>
-  <si>
-    <t>filter_running_status</t>
-  </si>
-  <si>
-    <t>offset</t>
-  </si>
-  <si>
-    <t>limit</t>
-  </si>
-  <si>
-    <t>sort_by</t>
-  </si>
-  <si>
-    <t>sort_mode</t>
-  </si>
-  <si>
-    <t>file_system_id_list</t>
-  </si>
-  <si>
-    <t>file_system_name_list</t>
-  </si>
-  <si>
-    <t>vstore_id</t>
-  </si>
-  <si>
-    <t>fs2</t>
-  </si>
-  <si>
-    <t>sp2</t>
   </si>
 </sst>
 </file>
@@ -576,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BD3"/>
+  <dimension ref="A1:BD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -756,27 +753,13 @@
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
         <v>70</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -790,49 +773,49 @@
     <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="K2:K1000" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Low,Middle,High"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="L2:L1000 N2:O1000 X2:X1000 AA2:AC1000 AE2:AG1000 AM2:AM1000 AQ2:AQ1000 AZ2:BA1000" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="L2:L1000 AZ2:BA1000 AQ2:AQ1000 AM2:AM1000 AE2:AG1000 AA2:AC1000 X2:X1000 N2:O1000" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="M2:M1000" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"fast,deep"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="P2:P1000" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="P2:P1000" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"normal,worm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="Q2:Q1000" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="Q2:Q1000" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"compliance,enterprise"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="S2:S1000 U2:U1000 W2:W1000" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="S2:S1000 W2:W1000 U2:U1000" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"year,month,day"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="Z2:Z1000" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="Z2:Z1000" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"hour,day"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AD2:AD1000" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AD2:AD1000" xr:uid="{00000000-0002-0000-0000-000011000000}">
       <formula1>"off,hourly,daily"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AH2:AH1000" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AH2:AH1000" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>"4 KB,8 KB,16 KB,32 KB,64 KB"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AL2:AL1000" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AL2:AL1000" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>"on,off"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AN2:AN1000" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AN2:AN1000" xr:uid="{00000000-0002-0000-0000-000018000000}">
       <formula1>"1,2,4,8,16,32"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AO2:AO1000" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AO2:AO1000" xr:uid="{00000000-0002-0000-0000-000019000000}">
       <formula1>"database,virtual_machine"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AP2:AP1000" xr:uid="{00000000-0002-0000-0000-00000E000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AP2:AP1000" xr:uid="{00000000-0002-0000-0000-00001A000000}">
       <formula1>"off,grow,grow_shrink"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AW2:AW1000" xr:uid="{00000000-0002-0000-0000-00000F000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="AW2:AW1000" xr:uid="{00000000-0002-0000-0000-00001C000000}">
       <formula1>"autosize_first,delete_snap_first"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="BB2:BB1000" xr:uid="{00000000-0002-0000-0000-000010000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="BB2:BB1000" xr:uid="{00000000-0002-0000-0000-00001F000000}">
       <formula1>"NTFS,UNIX"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="BD2:BD1000" xr:uid="{00000000-0002-0000-0000-000011000000}">
+    <dataValidation type="list" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." sqref="BD2:BD1000" xr:uid="{00000000-0002-0000-0000-000020000000}">
       <formula1>"Performance Mode,Capacity Balance Mode,Directory Balance Mode,Directory Shuffle Mode"</formula1>
     </dataValidation>
   </dataValidations>
@@ -853,40 +836,40 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>63</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>64</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>65</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>66</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>67</v>
-      </c>
-      <c r="L1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>